<commit_message>
Replaced Repeat step by Repeat QC step in QC templates(sample and library) workflow action.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_QC_v4_12_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_QC_v4_12_0.xlsx
@@ -24,7 +24,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>UFG</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="H5" authorId="0">
@@ -274,7 +274,7 @@
     <t xml:space="preserve">NanoDrop</t>
   </si>
   <si>
-    <t xml:space="preserve">Repeat step - Move to next step and repeat current step</t>
+    <t xml:space="preserve">Repeat QC step - Repeat current QC step</t>
   </si>
   <si>
     <t xml:space="preserve">A04</t>
@@ -2022,7 +2022,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="27.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.6"/>
@@ -26096,7 +26096,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="45.2"/>
   </cols>
@@ -27044,7 +27044,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.5"/>

</xml_diff>